<commit_message>
added sra download script
</commit_message>
<xml_diff>
--- a/references/references.xlsx
+++ b/references/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kaede\Documents\GitHub\MICB405_FINAL\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CC0104-7905-4A21-855D-CDDB7A0E790B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E52DD38-3D47-4F2D-B195-9DF7FEED36B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1770" windowWidth="20895" windowHeight="13380" xr2:uid="{ECE3871F-8FAF-4FA8-A80F-84D87A1911CF}"/>
+    <workbookView xWindow="6510" yWindow="1770" windowWidth="18690" windowHeight="13380" xr2:uid="{ECE3871F-8FAF-4FA8-A80F-84D87A1911CF}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="1" r:id="rId1"/>
@@ -295,9 +295,9 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BF24C791-AF89-4190-8712-F398878CB35A}" name="Checked?" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{E3AFC5FC-6F48-4FA2-ABE6-8E81200ED29C}" name="included?" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{58AA37F2-B196-4DD6-9CB9-2211F580CA25}" name="paper downloaded?" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{151D88C1-A2E4-43BA-AD42-F6BE82183D3D}" name="BioProject" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{E3AFC5FC-6F48-4FA2-ABE6-8E81200ED29C}" name="included?" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{58AA37F2-B196-4DD6-9CB9-2211F580CA25}" name="paper downloaded?" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{151D88C1-A2E4-43BA-AD42-F6BE82183D3D}" name="BioProject" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{1CCC792F-4878-4298-9E3D-2EF5EBA4B163}" name="Gene Expression Omnibus"/>
     <tableColumn id="5" xr3:uid="{D9E35F0D-5B40-4982-8F99-1AB3F004E096}" name="DOI"/>
     <tableColumn id="6" xr3:uid="{A08608B0-955E-42DB-9741-100297C306B3}" name="description"/>

</xml_diff>